<commit_message>
Re-parse data & regenerate all survey-answer sheets
</commit_message>
<xml_diff>
--- a/results/answers_q01.xlsx
+++ b/results/answers_q01.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,21 +484,21 @@
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>45840.78521831499</v>
+        <v>45854.64411551836</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>43faa0b9</t>
+          <t>2c1001cb</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4.642857142857143</v>
+        <v>7.405797101449275</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>3-5</t>
+          <t>6-10</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -507,17 +507,17 @@
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>45840.78521831499</v>
+        <v>45854.64411551836</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>5da96769</t>
+          <t>37cc37bf</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.5</v>
+        <v>2.881578947368421</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -530,21 +530,21 @@
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>45840.78521831499</v>
+        <v>45854.64411551836</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>6ca3e2f6</t>
+          <t>43faa0b9</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2.5</v>
+        <v>4.642857142857143</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1-2</t>
+          <t>3-5</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -553,17 +553,17 @@
         </is>
       </c>
       <c r="E5" s="2" t="n">
-        <v>45840.78521831499</v>
+        <v>45854.64411551836</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>790a4fcb</t>
+          <t>4abe3e88</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.666666666666667</v>
+        <v>2.836065573770492</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -576,21 +576,21 @@
         </is>
       </c>
       <c r="E6" s="2" t="n">
-        <v>45840.78521831499</v>
+        <v>45854.64411551836</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ad58f9da</t>
+          <t>50164f59</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.39622641509434</v>
+        <v>5.769230769230769</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>1-2</t>
+          <t>3-5</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -599,17 +599,17 @@
         </is>
       </c>
       <c r="E7" s="2" t="n">
-        <v>45840.78521831499</v>
+        <v>45854.64411551836</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>c02a1ce7</t>
+          <t>5cf70f79</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2.5</v>
+        <v>2.571428571428572</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -622,30 +622,375 @@
         </is>
       </c>
       <c r="E8" s="2" t="n">
-        <v>45840.78521831499</v>
+        <v>45854.64411551836</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>5da96769</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1-2</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>q01_sessions_avg_per_week</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>45854.64411551836</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>6ca3e2f6</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1-2</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>q01_sessions_avg_per_week</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>45854.64411551836</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>790a4fcb</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1.666666666666667</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>1-2</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>q01_sessions_avg_per_week</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>45854.64411551836</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>802cc63a</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2.910714285714286</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>1-2</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>q01_sessions_avg_per_week</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>45854.64411551836</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>85c3ea4d</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>9.839285714285714</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>6-10</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>q01_sessions_avg_per_week</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>45854.64411551836</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>942dfafb</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>8.027027027027026</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>6-10</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>q01_sessions_avg_per_week</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>45854.64411551836</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>9bc6ba8c</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>1-2</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>q01_sessions_avg_per_week</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>45854.64411551836</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>a2d65af2</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>1-2</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>q01_sessions_avg_per_week</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>45854.64411551836</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>a46f1771</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>3.28125</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>3-5</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>q01_sessions_avg_per_week</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>45854.64411551836</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ad58f9da</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>2.39622641509434</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>1-2</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>q01_sessions_avg_per_week</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>45854.64411551836</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>c7d9a301</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>3.848484848484849</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>3-5</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>q01_sessions_avg_per_week</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>45854.64411551836</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>ce8732ff</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>2.985714285714286</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>1-2</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>q01_sessions_avg_per_week</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>45854.64411551836</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>d6f1d567</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1.727272727272727</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>1-2</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>q01_sessions_avg_per_week</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>45854.64411551836</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
           <t>da9326c9</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="B22" t="n">
         <v>2.857142857142857</v>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>1-2</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>q01_sessions_avg_per_week</t>
-        </is>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>45840.78521831499</v>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>1-2</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>q01_sessions_avg_per_week</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>45854.64411551836</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>e09ca7bf</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>8.027027027027026</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>6-10</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>q01_sessions_avg_per_week</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>45854.64411551836</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>ef53a641</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>7.475247524752476</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>6-10</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>q01_sessions_avg_per_week</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>45854.64411551836</v>
       </c>
     </row>
   </sheetData>

</xml_diff>